<commit_message>
Integrando codigo de archivo tolerancia en el codigo master, faltan algunos log message y probar el codigo a full
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13290" activeTab="1"/>
+    <workbookView xWindow="20376" yWindow="-120" windowWidth="21840" windowHeight="13296" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="178">
   <si>
     <t>Name</t>
   </si>
@@ -554,6 +554,12 @@
   </si>
   <si>
     <t>C:\Users\ROBTIRELEO\AppData\Local\Apps\2.0\3B7TL0XA.NTH\L72C3K1L.7RV\ejec..tion_0a8a34db63dae999_0001.0000_dfe84433c170a406\EjecutarEpicorLeo.exe</t>
+  </si>
+  <si>
+    <t>C:\Users\ROBTIRELEO\Documents\JACK3\lib\net45\Data\Subsidiados</t>
+  </si>
+  <si>
+    <t>Subsidiados</t>
   </si>
 </sst>
 </file>
@@ -1103,25 +1109,25 @@
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="118" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75">
+    <row r="1" spans="1:1" ht="18">
       <c r="A1" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="18.75">
+    <row r="2" spans="1:1" ht="18">
       <c r="A2" s="7"/>
     </row>
-    <row r="3" spans="1:1" ht="60">
+    <row r="3" spans="1:1" ht="43.2">
       <c r="A3" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75">
+    <row r="4" spans="1:1" ht="15.6">
       <c r="A4" s="12" t="s">
         <v>52</v>
       </c>
@@ -1131,32 +1137,32 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75">
+    <row r="6" spans="1:1" ht="15.6">
       <c r="A6" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="45">
+    <row r="7" spans="1:1" ht="43.2">
       <c r="A7" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75">
+    <row r="8" spans="1:1" ht="15.6">
       <c r="A8" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="45">
+    <row r="9" spans="1:1" ht="43.2">
       <c r="A9" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="45">
+    <row r="10" spans="1:1" ht="43.2">
       <c r="A10" s="13" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="60">
+    <row r="11" spans="1:1" ht="43.2">
       <c r="A11" s="13" t="s">
         <v>61</v>
       </c>
@@ -1166,22 +1172,22 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.75">
+    <row r="13" spans="1:1" ht="15.6">
       <c r="A13" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="45">
+    <row r="14" spans="1:1" ht="43.2">
       <c r="A14" s="13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.75">
+    <row r="15" spans="1:1" ht="15.6">
       <c r="A15" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="30">
+    <row r="16" spans="1:1" ht="28.8">
       <c r="A16" s="13" t="s">
         <v>64</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="30">
+    <row r="19" spans="1:1" ht="28.8">
       <c r="A19" s="14" t="s">
         <v>46</v>
       </c>
@@ -1229,17 +1235,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z986"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="140.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="140.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1681,7 +1687,14 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A42" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>176</v>
+      </c>
+    </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2676,11 +2689,11 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="147.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="147.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2763,12 +2776,12 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="3" max="3" width="169.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="70.109375" customWidth="1"/>
+    <col min="3" max="3" width="169.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3791,14 +3804,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3888,12 +3901,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" customWidth="1"/>
+    <col min="2" max="2" width="63.5546875" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -5068,11 +5081,11 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="65.42578125" customWidth="1"/>
-    <col min="3" max="3" width="69.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="2" width="65.44140625" customWidth="1"/>
+    <col min="3" max="3" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Integracion completada, solucionando error con selector
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="183">
   <si>
     <t>Name</t>
   </si>
@@ -560,6 +560,21 @@
   </si>
   <si>
     <t>Subsidiados</t>
+  </si>
+  <si>
+    <t>RutaTolerancia</t>
+  </si>
+  <si>
+    <t>RutaTemplateTol</t>
+  </si>
+  <si>
+    <t>C:\Users\ROBTIRELEO\Documents\JACK3\lib\net45\Data\Tolerancia</t>
+  </si>
+  <si>
+    <t>C:\Users\ROBTIRELEO\Documents\JACK3\lib\net45\Data\Templates\Template Tolerancia.xlsx</t>
+  </si>
+  <si>
+    <t>ValorRango</t>
   </si>
 </sst>
 </file>
@@ -1233,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z986"/>
+  <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1359,46 +1374,42 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>120</v>
-      </c>
-    </row>
+    <row r="10" spans="1:26" ht="15" customHeight="1">
+      <c r="A10" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="21"/>
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1">
+      <c r="A11" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" s="21"/>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="23" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C14" s="23" t="s">
         <v>120</v>
@@ -1406,10 +1417,10 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C15" s="23" t="s">
         <v>120</v>
@@ -1417,10 +1428,10 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="23" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C16" s="23" t="s">
         <v>120</v>
@@ -1428,10 +1439,10 @@
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>120</v>
@@ -1439,10 +1450,10 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="23" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C18" s="23" t="s">
         <v>120</v>
@@ -1450,10 +1461,10 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="23" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C19" s="23" t="s">
         <v>120</v>
@@ -1461,10 +1472,10 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="23" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="C20" s="23" t="s">
         <v>120</v>
@@ -1472,157 +1483,161 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="23" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>133</v>
+        <v>101</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="23" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>129</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>134</v>
+        <v>114</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="23" t="s">
-        <v>70</v>
+        <v>127</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>71</v>
+        <v>137</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="23" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>111</v>
+        <v>129</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" s="23" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" s="23" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" s="23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" s="23" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" s="23" t="s">
-        <v>145</v>
+        <v>73</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>150</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" s="23" t="s">
-        <v>146</v>
+        <v>86</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" s="23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" s="23" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="B33" s="23"/>
+        <v>147</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>148</v>
+      </c>
       <c r="C33" s="23" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="B34" s="23"/>
+        <v>154</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>153</v>
+      </c>
       <c r="C34" s="23" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" s="23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B35" s="23"/>
       <c r="C35" s="23" t="s">
@@ -1631,7 +1646,7 @@
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" s="23" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B36" s="23"/>
       <c r="C36" s="23" t="s">
@@ -1640,7 +1655,7 @@
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1">
       <c r="A37" s="23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B37" s="23"/>
       <c r="C37" s="23" t="s">
@@ -1649,7 +1664,7 @@
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" s="23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B38" s="23"/>
       <c r="C38" s="23" t="s">
@@ -1658,7 +1673,7 @@
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" s="23" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="B39" s="23"/>
       <c r="C39" s="23" t="s">
@@ -1667,37 +1682,60 @@
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="B40" s="23" t="s">
-        <v>172</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="B40" s="23"/>
       <c r="C40" s="23" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" s="23" t="s">
-        <v>173</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>174</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="B41" s="23"/>
       <c r="C41" s="23" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A43" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A44" s="23" t="s">
         <v>177</v>
       </c>
-      <c r="B42" s="23" t="s">
+      <c r="B44" s="23" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A45" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="B45" s="23">
+        <v>10000</v>
+      </c>
+    </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2639,6 +2677,9 @@
     <row r="984" ht="14.25" customHeight="1"/>
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
+    <row r="987" ht="14.25" customHeight="1"/>
+    <row r="988" ht="14.25" customHeight="1"/>
+    <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se hicieron correcciones para el envio de correos electronicos en el config y se implemento el verificador de los check box. CODIGO LISTO PARA SUBIR A PRODUCTIVO, falta prueba de un patron
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="184">
   <si>
     <t>Name</t>
   </si>
@@ -535,9 +535,6 @@
     <t>UsuarioERRORcorg</t>
   </si>
   <si>
-    <t>http://leonisavirtual.leonisa.com/MessengerServices/rest/email/sendMultipleEmailStreamAttachment</t>
-  </si>
-  <si>
     <t>Informativo,Informativo,Warning,Error,Fatal</t>
   </si>
   <si>
@@ -575,6 +572,12 @@
   </si>
   <si>
     <t>ValorRango</t>
+  </si>
+  <si>
+    <t>gonzoas@gmail.com</t>
+  </si>
+  <si>
+    <t>https://leonisavirtual.leonisa.com/MessengerServices/rest/email/sendMultipleEmailStreamAttachment</t>
   </si>
 </sst>
 </file>
@@ -1250,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1324,7 +1327,7 @@
         <v>75</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>72</v>
@@ -1376,19 +1379,19 @@
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
       <c r="A10" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C10" s="21"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
       <c r="A11" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C11" s="21"/>
     </row>
@@ -1563,7 +1566,7 @@
         <v>78</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C28" s="23" t="s">
         <v>116</v>
@@ -1596,7 +1599,7 @@
         <v>145</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="C31" s="23" t="s">
         <v>150</v>
@@ -1648,7 +1651,9 @@
       <c r="A36" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="B36" s="23"/>
+      <c r="B36" s="23" t="s">
+        <v>182</v>
+      </c>
       <c r="C36" s="23" t="s">
         <v>157</v>
       </c>
@@ -1700,10 +1705,10 @@
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="23" t="s">
         <v>171</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>172</v>
       </c>
       <c r="C42" s="23" t="s">
         <v>157</v>
@@ -1711,10 +1716,10 @@
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="23" t="s">
         <v>173</v>
-      </c>
-      <c r="B43" s="23" t="s">
-        <v>174</v>
       </c>
       <c r="C43" s="23" t="s">
         <v>157</v>
@@ -1722,18 +1727,18 @@
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1">
       <c r="A44" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" s="24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B45" s="23">
-        <v>10000</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2681,8 +2686,11 @@
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B31" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
@@ -2797,7 +2805,7 @@
         <v>75</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>161</v>

</xml_diff>